<commit_message>
todos und anforderungen in readme aktualisiert
</commit_message>
<xml_diff>
--- a/TB-GI-Ist-Zustand.xlsx
+++ b/TB-GI-Ist-Zustand.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Eigene Dateien\tumorboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxst\Desktop\tumorboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBE07E4-3D34-4AA7-A0AC-26CFFCD91192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-2430" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TB-GI-Ist-Zustand" sheetId="1" r:id="rId1"/>
@@ -422,7 +423,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1228,11 +1229,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,7 +1926,7 @@
         <v>78</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1939,7 +1940,7 @@
         <v>78</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1953,7 +1954,7 @@
         <v>78</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1964,7 +1965,7 @@
         <v>46</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1975,7 +1976,7 @@
         <v>51</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>